<commit_message>
Replace more country names with three letter codes
</commit_message>
<xml_diff>
--- a/data/membership.xlsx
+++ b/data/membership.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">Australia National Plant Biosecurity Diagnostic Network</t>
   </si>
   <si>
-    <t xml:space="preserve">Australia</t>
+    <t xml:space="preserve">AUS</t>
   </si>
   <si>
     <t xml:space="preserve">GRDC Communities of Practice: Field Crop Diseases</t>
@@ -254,8 +254,8 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>